<commit_message>
Organization of test code folders
</commit_message>
<xml_diff>
--- a/Gráficas/Comparación-TeóricoExperimental/Angulos-Teoricos-Angulos-Voltaje-Experimentales.xlsx
+++ b/Gráficas/Comparación-TeóricoExperimental/Angulos-Teoricos-Angulos-Voltaje-Experimentales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TG-II\Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TG-II\GitHub\Gráficas\Comparación-TeóricoExperimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C81A935-A3E5-4318-BA99-68CA83C1E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0126213A-3560-4045-82A0-BD814EF31B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{CC6BEE00-C615-41D4-A4AF-3C1181C6EB3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{CC6BEE00-C615-41D4-A4AF-3C1181C6EB3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -140,15 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1260,6 +1257,354 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GRADOS LINEALIZADOS M1</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja2!$F$2:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja2!$I$2:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>112.66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>165.76400000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>139.60300000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>159.393</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.372999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.369</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.495600000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110.033</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>162.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>146.25700000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.7988</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>126.07599999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110.36799999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>127.364</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.91900000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>82.083600000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>189.63399999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>160.12</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DE40-4801-BE7E-E4A91AF3D3D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GRADOS LINEALIZADOS M2</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja2!$F$2:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja2!$J$2:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>69.014799999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.857999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.020099999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.132400000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112.44799999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>115.857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.131900000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97.970200000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.65300000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.956400000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.313499999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46.039000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64.149299999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39.835799999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86.845600000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120.998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>112.783</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>118.372</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DE40-4801-BE7E-E4A91AF3D3D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
@@ -1611,392 +1956,7 @@
         </c:dLbls>
         <c:axId val="460019120"/>
         <c:axId val="291353840"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Hoja2!$I$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>GRADOS LINEALIZADOS M1</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent3"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Hoja2!$F$2:$F$19</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="18"/>
-                      <c:pt idx="0">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>12</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>15</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>18</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Hoja2!$I$2:$I$19</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="18"/>
-                      <c:pt idx="0">
-                        <c:v>112.66</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>165.76400000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>139.60300000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>159.393</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>56.372999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>83.369</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>49.495600000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>110.033</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>162.91399999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>146.25700000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>53.7988</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>126.07599999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>110.36799999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>127.364</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>181.91900000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>82.083600000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>189.63399999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>160.12</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-DE40-4801-BE7E-E4A91AF3D3D3}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="3"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Hoja2!$J$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>GRADOS LINEALIZADOS M2</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent4"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent4"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Hoja2!$F$2:$F$19</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="18"/>
-                      <c:pt idx="0">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>12</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>15</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>18</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Hoja2!$J$2:$J$19</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="18"/>
-                      <c:pt idx="0">
-                        <c:v>69.014799999999994</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>61.857999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>97.020099999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>70.132400000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>112.44799999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>115.857</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>97.131900000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>97.970200000000006</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>100.65300000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>77.956400000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>54.313499999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>46.039000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>64.149299999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>39.835799999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>86.845600000000005</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>120.998</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>112.783</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>118.372</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-DE40-4801-BE7E-E4A91AF3D3D3}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="460019120"/>
@@ -3698,7 +3658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B05BFD6-325E-4D0B-83EF-5D8CB2E3EB06}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3838,8 +3798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054ADC3A-F753-4F5F-A054-5BCDD3886A05}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="66" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView topLeftCell="A21" zoomScale="66" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,7 +3894,7 @@
         <f>+SQRT(POWER((((G2-I2)/G2)*100),2))</f>
         <v>0.46101852099551099</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="1">
         <f t="shared" ref="N2:N19" si="0">+SQRT(POWER((((G2-K2)/G2)*100),2))</f>
         <v>3.9975745253827735</v>
       </c>
@@ -3978,7 +3938,7 @@
         <f t="shared" ref="M3:M19" si="3">+SQRT(POWER((((G3-I3)/G3)*100),2))</f>
         <v>4.9743839806470938</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="1">
         <f t="shared" si="0"/>
         <v>1.8080033436979641</v>
       </c>
@@ -4022,7 +3982,7 @@
         <f t="shared" si="3"/>
         <v>3.5185157721455198</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="1">
         <f t="shared" si="0"/>
         <v>0.18908778122172615</v>
       </c>
@@ -4066,7 +4026,7 @@
         <f t="shared" si="3"/>
         <v>4.3052338136558221</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="1">
         <f t="shared" si="0"/>
         <v>1.0332822908895831</v>
       </c>
@@ -4110,7 +4070,7 @@
         <f t="shared" si="3"/>
         <v>5.7109022971395325</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="1">
         <f t="shared" si="0"/>
         <v>14.073868407055667</v>
       </c>
@@ -4154,7 +4114,7 @@
         <f t="shared" si="3"/>
         <v>1.2568962290744301</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>7.1789478172502257</v>
       </c>
@@ -4198,7 +4158,7 @@
         <f t="shared" si="3"/>
         <v>4.8355527527080895</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="1">
         <f>+SQRT(POWER((((G8-K8)/G8)*100),2))</f>
         <v>14.448977708390201</v>
       </c>
@@ -4242,7 +4202,7 @@
         <f t="shared" si="3"/>
         <v>1.5673605021461277</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>3.0479531084137101</v>
       </c>
@@ -4286,7 +4246,7 @@
         <f t="shared" si="3"/>
         <v>4.9257403423801716</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>1.7054603068282794</v>
       </c>
@@ -4330,7 +4290,7 @@
         <f t="shared" si="3"/>
         <v>3.6284151456751004</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="1">
         <f t="shared" si="0"/>
         <v>8.5732910100902199E-2</v>
       </c>
@@ -4374,7 +4334,7 @@
         <f t="shared" si="3"/>
         <v>5.2489384298095594</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="1">
         <f t="shared" si="0"/>
         <v>14.054995588165365</v>
       </c>
@@ -4418,7 +4378,7 @@
         <f t="shared" si="3"/>
         <v>3.3994636310700281</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="1">
         <f t="shared" si="0"/>
         <v>0.70121626165618589</v>
       </c>
@@ -4462,7 +4422,7 @@
         <f t="shared" si="3"/>
         <v>2.0659552037287021</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="1">
         <f t="shared" si="0"/>
         <v>2.5579373739989322</v>
       </c>
@@ -4506,7 +4466,7 @@
         <f t="shared" si="3"/>
         <v>2.2864347840054036</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="1">
         <f t="shared" si="0"/>
         <v>1.7290811696394803</v>
       </c>
@@ -4550,7 +4510,7 @@
         <f t="shared" si="3"/>
         <v>7.4035151937371344</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="1">
         <f t="shared" si="0"/>
         <v>4.4515553876218545</v>
       </c>
@@ -4594,7 +4554,7 @@
         <f t="shared" si="3"/>
         <v>0.19554852459737174</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="1">
         <f t="shared" si="0"/>
         <v>5.907713791175655</v>
       </c>
@@ -4638,7 +4598,7 @@
         <f t="shared" si="3"/>
         <v>7.4651056040711383</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="1">
         <f t="shared" si="0"/>
         <v>4.6316183179285924</v>
       </c>
@@ -4682,7 +4642,7 @@
         <f t="shared" si="3"/>
         <v>4.2651559549391234</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="1">
         <f t="shared" si="0"/>
         <v>1.0093117145275843</v>
       </c>

</xml_diff>